<commit_message>
add english version (#1237)
* add english version

* add more english doc

* refine

* refine

* refine

* refine

* refine

* refine format

* refine

* refine

* a little adjustment

* a little more adjustment

* support asset bundle in preview

* refine some english expression
</commit_message>
<xml_diff>
--- a/zh/asset-workflow/scene-managing/release-resources.xlsx
+++ b/zh/asset-workflow/scene-managing/release-resources.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12465" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="中文" sheetId="1" r:id="rId1"/>
@@ -38,27 +38,7 @@
     <t>不释放资源</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">当场景切换后，由于资源已经被释放，脚本中的引用可能会变成非法的，有可能引起渲染异常等问题。那么可以使用 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Avenir Book"/>
-        <charset val="134"/>
-      </rPr>
-      <t>cc.assetManager.finalizer.lock</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="黑体-简 细体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">    来保留这些脚本资源在场景切换时不被释放。</t>
-    </r>
+    <t>当场景切换后，由于资源已经被释放，脚本中的引用可能会变成非法的，有可能引起渲染异常等问题。那么可以使用 Asset.addRef 来保留这些脚本资源在场景切换时不被释放。</t>
   </si>
   <si>
     <t xml:space="preserve">该场景中直接或间接引用到的所有资源（脚本动态加载的不算），默认都会自动释放。
@@ -75,7 +55,7 @@
         <rFont val="Avenir Book"/>
         <charset val="134"/>
       </rPr>
-      <t>cc.assetManager.release</t>
+      <t>cc.assetManager.releaseAsset</t>
     </r>
     <r>
       <rPr>
@@ -143,12 +123,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Avenir Book"/>
-        <charset val="134"/>
-      </rPr>
       <t>When the scene is switched, the references in the script may become illegal because the resources have been freed, which can cause problems such as rendering exceptions. You can use '</t>
     </r>
     <r>
@@ -159,7 +133,7 @@
         <rFont val="Avenir Book"/>
         <charset val="134"/>
       </rPr>
-      <t>cc.loader.setAutoRelease'</t>
+      <t>Asset.addRef'</t>
     </r>
     <r>
       <rPr>
@@ -168,39 +142,14 @@
         <rFont val="Avenir Book"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> or '</t>
+      <t xml:space="preserve">  to keep these script resources from being freed when the scene is switched.</t>
     </r>
+  </si>
+  <si>
+    <t>All assets (directly or indirectly) referenced by current scene (except loaded dynamically in scripts) will release by default.</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Avenir Book"/>
-        <charset val="134"/>
-      </rPr>
-      <t>cc.loader.setAutoReleaseRecursively'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Avenir Book"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> to keep these script resources from being freed when the scene is switched.</t>
-    </r>
-  </si>
-  <si>
-    <t>All assets (directly or indirectly) referenced by current scene (except loaded dynamically in scripts) will release by default.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Avenir Book"/>
-        <charset val="134"/>
-      </rPr>
       <t>Invoke '</t>
     </r>
     <r>
@@ -211,7 +160,7 @@
         <rFont val="Avenir Book"/>
         <charset val="134"/>
       </rPr>
-      <t>cc.loader.release'</t>
+      <t>cc.assetManager.releaseAsset'</t>
     </r>
     <r>
       <rPr>
@@ -236,11 +185,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="33">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -304,33 +253,13 @@
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="黑体-简 细体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color rgb="FF24292E"/>
       <name val="黑体-简 细体"/>
       <charset val="136"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -339,7 +268,29 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -350,15 +301,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,16 +325,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,6 +341,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -403,56 +393,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -473,12 +416,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Avenir Book"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF24292E"/>
@@ -495,67 +432,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,115 +606,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -874,8 +811,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -895,35 +847,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -945,6 +888,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -953,166 +905,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1224,10 +1161,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1236,7 +1173,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1561,7 +1498,7 @@
   <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1653,7 +1590,7 @@
   <dimension ref="B1:G8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="7" outlineLevelCol="6"/>

</xml_diff>